<commit_message>
demo ppt done :)
</commit_message>
<xml_diff>
--- a/data/PWM to curent driver voltage out.xlsx
+++ b/data/PWM to curent driver voltage out.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cd3e99d6a3c3959/Documents/2018 UBC/ELEC 391/Controller/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucyl\Documents\GitHub\Controller\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{67FEEA24-0DC0-41B5-92AE-B3DBDCD37BB9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{38EC138A-27A1-457E-8123-7AB6BEF8601F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C298EA-0096-48FE-9086-7F41299E4DE0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="10440" activeTab="1" xr2:uid="{BE8C3103-C611-45FC-8490-5115FA256B11}"/>
   </bookViews>
@@ -185,6 +185,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>PWM to Average Voltage Supplied</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -409,6 +434,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>PWM</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -449,6 +529,7 @@
         <c:crossAx val="596546256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="596546256"/>
@@ -471,6 +552,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> Voltage (V)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -511,6 +652,7 @@
         <c:crossAx val="596544616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -520,37 +662,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1155,16 +1266,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>148590</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>483870</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1495,21 +1606,21 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1529,7 +1640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1543,7 +1654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
         <v>1.41</v>
       </c>
@@ -1554,7 +1665,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
         <v>2</v>
       </c>
@@ -1565,7 +1676,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
         <v>3</v>
       </c>
@@ -1576,7 +1687,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
         <v>4</v>
       </c>
@@ -1587,32 +1698,32 @@
         <v>340</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
         <v>12</v>
       </c>
@@ -1626,25 +1737,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1E732A-C1D6-4834-B255-E8E2D095B619}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.89453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1664,7 +1775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1684,7 +1795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
         <v>10</v>
       </c>
@@ -1707,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
         <v>20</v>
       </c>
@@ -1730,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
         <v>30</v>
       </c>
@@ -1761,7 +1872,7 @@
         <v>0.37416666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
         <v>35</v>
       </c>
@@ -1773,7 +1884,7 @@
         <v>0.40916666666666668</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H16" si="1">1-F8</f>
+        <f t="shared" ref="H8:H15" si="1">1-F8</f>
         <v>0.59083333333333332</v>
       </c>
       <c r="I8">
@@ -1781,7 +1892,7 @@
         <v>0.32500000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
         <v>40</v>
       </c>
@@ -1801,7 +1912,7 @@
         <v>0.255</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <v>50</v>
       </c>
@@ -1812,15 +1923,15 @@
         <v>255</v>
       </c>
       <c r="E10">
-        <f>D10*6000/400</f>
+        <f t="shared" ref="E10:E15" si="3">D10*6000/400</f>
         <v>3825</v>
       </c>
       <c r="F10">
-        <f>C10/12</f>
+        <f t="shared" ref="F10:F15" si="4">C10/12</f>
         <v>0.52249999999999996</v>
       </c>
       <c r="G10">
-        <f>E10/$E$15</f>
+        <f t="shared" ref="G10:G15" si="5">E10/$E$15</f>
         <v>0.63118811881188119</v>
       </c>
       <c r="H10">
@@ -1832,7 +1943,7 @@
         <v>0.21166666666666678</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <v>80</v>
       </c>
@@ -1843,15 +1954,15 @@
         <v>326</v>
       </c>
       <c r="E11">
-        <f>D11*6000/400</f>
+        <f t="shared" si="3"/>
         <v>4890</v>
       </c>
       <c r="F11">
-        <f>C11/12</f>
+        <f t="shared" si="4"/>
         <v>0.61833333333333329</v>
       </c>
       <c r="G11">
-        <f>E11/$E$15</f>
+        <f t="shared" si="5"/>
         <v>0.80693069306930698</v>
       </c>
       <c r="H11">
@@ -1863,7 +1974,7 @@
         <v>0.11583333333333345</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
         <v>120</v>
       </c>
@@ -1874,15 +1985,15 @@
         <v>367</v>
       </c>
       <c r="E12">
-        <f>D12*6000/400</f>
+        <f t="shared" si="3"/>
         <v>5505</v>
       </c>
       <c r="F12">
-        <f>C12/12</f>
+        <f t="shared" si="4"/>
         <v>0.67249999999999999</v>
       </c>
       <c r="G12">
-        <f>E12/$E$15</f>
+        <f t="shared" si="5"/>
         <v>0.90841584158415845</v>
       </c>
       <c r="H12">
@@ -1894,7 +2005,7 @@
         <v>6.1666666666666758E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B13">
         <v>150</v>
       </c>
@@ -1905,15 +2016,15 @@
         <v>381</v>
       </c>
       <c r="E13">
-        <f>D13*6000/400</f>
+        <f t="shared" si="3"/>
         <v>5715</v>
       </c>
       <c r="F13">
-        <f>C13/12</f>
+        <f t="shared" si="4"/>
         <v>0.69416666666666671</v>
       </c>
       <c r="G13">
-        <f>E13/$E$15</f>
+        <f t="shared" si="5"/>
         <v>0.94306930693069302</v>
       </c>
       <c r="H13">
@@ -1925,7 +2036,7 @@
         <v>4.0000000000000036E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B14">
         <v>200</v>
       </c>
@@ -1936,15 +2047,15 @@
         <v>392</v>
       </c>
       <c r="E14">
-        <f>D14*6000/400</f>
+        <f t="shared" si="3"/>
         <v>5880</v>
       </c>
       <c r="F14">
-        <f>C14/12</f>
+        <f t="shared" si="4"/>
         <v>0.72000000000000008</v>
       </c>
       <c r="G14">
-        <f>E14/$E$15</f>
+        <f t="shared" si="5"/>
         <v>0.97029702970297027</v>
       </c>
       <c r="H14">
@@ -1956,7 +2067,7 @@
         <v>1.4166666666666661E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B15">
         <v>255</v>
       </c>
@@ -1967,15 +2078,15 @@
         <v>404</v>
       </c>
       <c r="E15">
-        <f>D15*6000/400</f>
+        <f t="shared" si="3"/>
         <v>6060</v>
       </c>
       <c r="F15">
-        <f>C15/12</f>
+        <f t="shared" si="4"/>
         <v>0.73416666666666675</v>
       </c>
       <c r="G15">
-        <f>E15/$E$15</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H15">

</xml_diff>

<commit_message>
Added header for finalized pin config
</commit_message>
<xml_diff>
--- a/data/PWM to curent driver voltage out.xlsx
+++ b/data/PWM to curent driver voltage out.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucyl\Documents\GitHub\Controller\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cd3e99d6a3c3959/Documents/2018 UBC/ELEC 391/Controller/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C298EA-0096-48FE-9086-7F41299E4DE0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="6_{5366F0F5-A851-408A-B9B1-69CCDF44F802}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{28EB8811-4B6C-4A11-805D-1DFB06E9F7F6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="10440" activeTab="1" xr2:uid="{BE8C3103-C611-45FC-8490-5115FA256B11}"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="23040" windowHeight="10440" activeTab="1" xr2:uid="{BE8C3103-C611-45FC-8490-5115FA256B11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1266,16 +1266,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>148590</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>232410</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>483870</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>567690</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1606,21 +1606,21 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1.41</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>3</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>4</v>
       </c>
@@ -1698,32 +1698,32 @@
         <v>340</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>12</v>
       </c>
@@ -1738,24 +1738,24 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>10</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>20</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>30</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>0.37416666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>35</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>0.32500000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>40</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>0.255</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>50</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>0.21166666666666678</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>80</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>0.11583333333333345</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>120</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>6.1666666666666758E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>150</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>4.0000000000000036E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>200</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>1.4166666666666661E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>255</v>
       </c>

</xml_diff>